<commit_message>
Fixed princeton language info- entered in Excel as a percentage- causing problems.
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/babylab_princeton_participants_BL.xlsx
+++ b/processed_data/participants_cleaned/babylab_princeton_participants_BL.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/lew-williams/Studies/ManyBabies/2 Data/2c Processed data/FINAL/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDFB7CE-FDC7-554C-AE2B-F76DC55CE2D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3020" yWindow="620" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Variable explanations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -631,7 +625,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d"/>
   </numFmts>
@@ -797,13 +791,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1153,14 +1147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="9.5" customWidth="1"/>
@@ -1180,13 +1174,13 @@
     <col min="32" max="32" width="18.6640625" customWidth="1"/>
     <col min="33" max="33" width="16.1640625" customWidth="1"/>
     <col min="34" max="43" width="10.6640625" customWidth="1"/>
-    <col min="44" max="44" width="10.6640625" style="20" customWidth="1"/>
+    <col min="44" max="44" width="20.6640625" style="19" customWidth="1"/>
     <col min="45" max="47" width="10.6640625" customWidth="1"/>
     <col min="51" max="51" width="15" customWidth="1"/>
     <col min="59" max="59" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:60" ht="12">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -1364,9 +1358,9 @@
       <c r="BG1" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="BH1" s="20"/>
-    </row>
-    <row r="2" spans="1:60" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="BH1" s="19"/>
+    </row>
+    <row r="2" spans="1:60" s="19" customFormat="1" ht="12">
       <c r="A2" s="18" t="s">
         <v>121</v>
       </c>
@@ -1401,8 +1395,8 @@
       <c r="L2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="M2" s="19">
-        <v>0.7</v>
+      <c r="M2" s="23">
+        <v>70</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>137</v>
@@ -1544,7 +1538,7 @@
       </c>
       <c r="BH2" s="16"/>
     </row>
-    <row r="3" spans="1:60" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:60" s="19" customFormat="1" ht="12">
       <c r="A3" s="18" t="s">
         <v>121</v>
       </c>
@@ -1721,7 +1715,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:60" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:60" s="19" customFormat="1" ht="12">
       <c r="A4" s="18" t="s">
         <v>121</v>
       </c>
@@ -1899,7 +1893,7 @@
       </c>
       <c r="BH4" s="16"/>
     </row>
-    <row r="5" spans="1:60" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:60" s="19" customFormat="1" ht="12">
       <c r="A5" s="18" t="s">
         <v>121</v>
       </c>
@@ -2060,7 +2054,7 @@
       <c r="BB5" s="16">
         <v>3</v>
       </c>
-      <c r="BC5" s="21" t="s">
+      <c r="BC5" s="20" t="s">
         <v>156</v>
       </c>
       <c r="BD5" s="16" t="s">
@@ -2077,7 +2071,7 @@
       </c>
       <c r="BH5" s="16"/>
     </row>
-    <row r="6" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A6" s="18" t="s">
         <v>121</v>
       </c>
@@ -2223,7 +2217,7 @@
       <c r="AW6" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX6" s="22" t="s">
+      <c r="AX6" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY6" s="16">
@@ -2238,7 +2232,7 @@
       <c r="BB6" s="16">
         <v>1</v>
       </c>
-      <c r="BC6" s="21" t="s">
+      <c r="BC6" s="20" t="s">
         <v>167</v>
       </c>
       <c r="BD6" s="16" t="s">
@@ -2254,7 +2248,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A7" s="18" t="s">
         <v>121</v>
       </c>
@@ -2400,7 +2394,7 @@
       <c r="AW7" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX7" s="22" t="s">
+      <c r="AX7" s="21" t="s">
         <v>165</v>
       </c>
       <c r="AY7" s="16">
@@ -2431,7 +2425,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A8" s="18" t="s">
         <v>121</v>
       </c>
@@ -2577,7 +2571,7 @@
       <c r="AW8" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX8" s="23" t="s">
+      <c r="AX8" s="22" t="s">
         <v>165</v>
       </c>
       <c r="AY8" s="16">
@@ -2608,7 +2602,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A9" s="18" t="s">
         <v>121</v>
       </c>
@@ -2754,7 +2748,7 @@
       <c r="AW9" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX9" s="22" t="s">
+      <c r="AX9" s="21" t="s">
         <v>165</v>
       </c>
       <c r="AY9" s="16">
@@ -2785,7 +2779,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A10" s="18" t="s">
         <v>121</v>
       </c>
@@ -2931,7 +2925,7 @@
       <c r="AW10" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX10" s="22" t="s">
+      <c r="AX10" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY10" s="16">
@@ -2962,7 +2956,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A11" s="18" t="s">
         <v>121</v>
       </c>
@@ -3108,7 +3102,7 @@
       <c r="AW11" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX11" s="22" t="s">
+      <c r="AX11" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY11" s="16">
@@ -3139,7 +3133,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A12" s="18" t="s">
         <v>121</v>
       </c>
@@ -3285,7 +3279,7 @@
       <c r="AW12" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX12" s="22" t="s">
+      <c r="AX12" s="21" t="s">
         <v>172</v>
       </c>
       <c r="AY12" s="16">
@@ -3316,7 +3310,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A13" s="18" t="s">
         <v>121</v>
       </c>
@@ -3462,7 +3456,7 @@
       <c r="AW13" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX13" s="22" t="s">
+      <c r="AX13" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY13" s="16">
@@ -3493,7 +3487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A14" s="18" t="s">
         <v>121</v>
       </c>
@@ -3639,7 +3633,7 @@
       <c r="AW14" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX14" s="22" t="s">
+      <c r="AX14" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY14" s="16">
@@ -3670,7 +3664,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A15" s="18" t="s">
         <v>121</v>
       </c>
@@ -3816,7 +3810,7 @@
       <c r="AW15" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX15" s="22" t="s">
+      <c r="AX15" s="21" t="s">
         <v>172</v>
       </c>
       <c r="AY15" s="16">
@@ -3847,7 +3841,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:60" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:60" s="19" customFormat="1" ht="13">
       <c r="A16" s="18" t="s">
         <v>121</v>
       </c>
@@ -3993,7 +3987,7 @@
       <c r="AW16" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX16" s="22" t="s">
+      <c r="AX16" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY16" s="16">
@@ -4024,7 +4018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:59" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:59" s="19" customFormat="1" ht="13">
       <c r="A17" s="18" t="s">
         <v>121</v>
       </c>
@@ -4170,7 +4164,7 @@
       <c r="AW17" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX17" s="22" t="s">
+      <c r="AX17" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY17" s="16">
@@ -4201,7 +4195,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:59" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:59" s="19" customFormat="1" ht="13">
       <c r="A18" s="18" t="s">
         <v>121</v>
       </c>
@@ -4217,7 +4211,7 @@
       <c r="E18" s="18">
         <v>218</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <v>2</v>
       </c>
       <c r="G18" s="16" t="s">
@@ -4347,7 +4341,7 @@
       <c r="AW18" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX18" s="22" t="s">
+      <c r="AX18" s="21" t="s">
         <v>165</v>
       </c>
       <c r="AY18" s="16">
@@ -4378,7 +4372,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:59" s="20" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:59" s="19" customFormat="1" ht="12">
       <c r="A19" s="16" t="s">
         <v>121</v>
       </c>
@@ -4394,7 +4388,7 @@
       <c r="E19" s="18">
         <v>212</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="19">
         <v>4</v>
       </c>
       <c r="G19" s="16" t="s">
@@ -4555,7 +4549,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:59" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:59" s="19" customFormat="1" ht="13">
       <c r="A20" s="16" t="s">
         <v>121</v>
       </c>
@@ -4571,7 +4565,7 @@
       <c r="E20" s="18">
         <v>191</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="19">
         <v>1</v>
       </c>
       <c r="G20" s="16" t="s">
@@ -4701,7 +4695,7 @@
       <c r="AW20" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AX20" s="22" t="s">
+      <c r="AX20" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AY20" s="16">
@@ -4732,7 +4726,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:59" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:59" ht="13">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -4793,7 +4787,7 @@
       <c r="BF21" s="4"/>
       <c r="BG21" s="4"/>
     </row>
-    <row r="22" spans="1:59" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:59" ht="13">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -4853,7 +4847,7 @@
       <c r="BF22" s="4"/>
       <c r="BG22" s="4"/>
     </row>
-    <row r="23" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:59" ht="15.75" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -4914,7 +4908,7 @@
       <c r="BF23" s="4"/>
       <c r="BG23" s="4"/>
     </row>
-    <row r="24" spans="1:59" ht="14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:59" ht="13">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -4975,7 +4969,7 @@
       <c r="BF24" s="4"/>
       <c r="BG24" s="4"/>
     </row>
-    <row r="25" spans="1:59" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:59" ht="13">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5036,7 +5030,7 @@
       <c r="BF25" s="4"/>
       <c r="BG25" s="4"/>
     </row>
-    <row r="26" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:59" ht="15.75" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -5097,7 +5091,7 @@
       <c r="BF26" s="4"/>
       <c r="BG26" s="4"/>
     </row>
-    <row r="27" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:59" ht="15.75" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -5158,7 +5152,7 @@
       <c r="BF27" s="4"/>
       <c r="BG27" s="4"/>
     </row>
-    <row r="28" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:59" ht="15.75" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -5218,7 +5212,7 @@
       <c r="BF28" s="4"/>
       <c r="BG28" s="4"/>
     </row>
-    <row r="29" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:59" ht="15.75" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -5278,7 +5272,7 @@
       <c r="BF29" s="4"/>
       <c r="BG29" s="4"/>
     </row>
-    <row r="30" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:59" ht="15.75" customHeight="1">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5339,7 +5333,7 @@
       <c r="BF30" s="4"/>
       <c r="BG30" s="4"/>
     </row>
-    <row r="31" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:59" ht="15.75" customHeight="1">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -5399,7 +5393,7 @@
       <c r="BF31" s="4"/>
       <c r="BG31" s="4"/>
     </row>
-    <row r="32" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:59" ht="15.75" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -5459,7 +5453,7 @@
       <c r="BF32" s="4"/>
       <c r="BG32" s="4"/>
     </row>
-    <row r="33" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:59" ht="15.75" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -5532,7 +5526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -5540,14 +5534,14 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SqUJIwvswVa2-8W_ijJBIO2NE9AR7FI1Q9DT15vWlZE/edit?usp=sharing","GENERAL NOTE: please refer to the upload instructions for the most up to date version")</f>
         <v>GENERAL NOTE: please refer to the upload instructions for the most up to date version</v>
@@ -5557,14 +5551,14 @@
       <c r="D1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -5578,7 +5572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -5592,7 +5586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -5606,7 +5600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -5620,7 +5614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -5634,7 +5628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -5648,7 +5642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -5662,7 +5656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -5676,7 +5670,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -5690,7 +5684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -5704,7 +5698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -5718,7 +5712,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -5732,7 +5726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
@@ -5746,7 +5740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -5760,7 +5754,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -5774,7 +5768,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -5788,7 +5782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -5802,7 +5796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -5816,7 +5810,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
@@ -5830,7 +5824,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -5844,7 +5838,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
@@ -5858,7 +5852,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>60</v>
       </c>
@@ -5872,7 +5866,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
@@ -5886,7 +5880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
@@ -5900,7 +5894,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>67</v>
       </c>
@@ -5914,7 +5908,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>69</v>
       </c>
@@ -5928,7 +5922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>71</v>
       </c>
@@ -5942,7 +5936,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -5956,7 +5950,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
@@ -5970,7 +5964,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>79</v>
       </c>
@@ -5984,7 +5978,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>81</v>
       </c>
@@ -5998,7 +5992,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>83</v>
       </c>
@@ -6012,7 +6006,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>85</v>
       </c>
@@ -6026,7 +6020,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>87</v>
       </c>
@@ -6040,7 +6034,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>89</v>
       </c>
@@ -6054,7 +6048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>91</v>
       </c>
@@ -6068,7 +6062,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>93</v>
       </c>
@@ -6082,7 +6076,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>95</v>
       </c>
@@ -6096,7 +6090,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>97</v>
       </c>
@@ -6110,7 +6104,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>98</v>
       </c>
@@ -6124,7 +6118,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>99</v>
       </c>
@@ -6138,7 +6132,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>100</v>
       </c>
@@ -6152,7 +6146,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>101</v>
       </c>
@@ -6166,13 +6160,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
       <c r="C48" s="13"/>
     </row>
   </sheetData>

</xml_diff>